<commit_message>
update notes and codes
</commit_message>
<xml_diff>
--- a/@Core Java Notes/My Note's/MyJavaMemory.xlsx
+++ b/@Core Java Notes/My Note's/MyJavaMemory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\@Java Placement Course\Java\Code-with-Java\Code-with-Java\@Core Java Notes\My Note's\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF33BC89-BE58-41F7-9883-44E41A2A4A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C1AB6E-131B-4C4E-9AA4-3F7CCE0A6DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6F371268-58D1-405B-B7B9-1D6EE88827E6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>Shallow Copy (सरळ कॉपी)</t>
   </si>
@@ -440,12 +440,188 @@
 Constructor executed  
 Constructor executed</t>
   </si>
+  <si>
+    <t>Like saving a WhatsApp chat backup → The chats (objects) are converted into a file (bytes). Later, when you restore backup, it becomes original messages again (deserialization).</t>
+  </si>
+  <si>
+    <t>Serialization</t>
+  </si>
+  <si>
+    <r>
+      <t>Serialization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> म्हणजे object ला bytes मध्ये रूपांतरित करणे. हे bytes आपण फाईलमध्ये सेव्ह करू शकतो, नेटवर्कवर पाठवू शकतो किंवा database मध्ये ठेवू शकतो. परत object मध्ये बदलण्याला </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Deserialization</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> म्हणतात.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  तुझ्याकडे Student नावाचा object आहे:
+Student s1 = new Student(101, "Lalit");
+जर तुला हा object फाईलमध्ये सेव्ह करायचा असेल → Serialization वापर. नंतर फाईल वाचून परत Student object तयार करायचा असेल → Deserialization वापर.   Java मध्ये कसे करतात?
+ज्या class चे object serialize करायचे आहे त्याने Serializable interface implement केले पाहिजे.
+(हा एक marker interface आहे, methods नाहीत).
+Serialize करण्यासाठी → ObjectOutputStream
+Deserialize करण्यासाठी → ObjectInputStream</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">👉 Serialization is the process of converting an object into a byte stream (a sequence of bytes) so that:
+It can be saved to a file or database
+It can be transmitted over a network (e.g., in distributed systems, RMI, messaging)
+Later, it can be reconstructed back into the same object using deserialization.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>How it works</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+To serialize an object, its class must implement the Serializable marker interface.
+Java provides</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ObjectOutputStream</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ObjectInputStream</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> classes for this.</t>
+    </r>
+  </si>
+  <si>
+    <t>Marker Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A marker interface is an empty interface(no methods or fields). It is used to give special informantion (metadata) to the JVM or frameworks that the class implementing is has a particular property. Examples: Serializable, cloneable, Remote. </t>
+  </si>
+  <si>
+    <t>Marker Interface म्हणजे एक रिकामे interface (त्यात methods/fields नसतात). हे class ला विशेष चिन्ह (mark) देण्यासाठी वापरले जाते जेणेकरून JVM किंवा framework त्या class ला वेगळ्या प्रकारे हाताळेल. उदा. Serializable, Cloneable, Remote.</t>
+  </si>
+  <si>
+    <t>✔ Example: A VIP pass in an event. The pass itself has no instructions (empty), but security recognizes that the person with this pass gets special treatment. Similarly, a marker interface marks a class for special behavior.</t>
+  </si>
+  <si>
+    <t>import java.io.*;
+class Student implements Serializable {
+    int id;
+    String name;
+    Student(int id, String name) {
+        this.id = id;
+        this.name = name;
+    }
+}
+public class Test {
+    public static void main(String[] args) throws Exception {
+        // Object तयार केला
+        Student s1 = new Student(101, "Lalit");
+        // ---- Serialization (फाईल मध्ये लिहिले) ----
+        FileOutputStream fos = new FileOutputStream("student.ser");
+        ObjectOutputStream oos = new ObjectOutputStream(fos);
+        oos.writeObject(s1);
+        oos.close();
+        System.out.println("Object Serialize झाला!");
+        // ---- Deserialization (फाईल मधून वाचले) ----
+        FileInputStream fis = new FileInputStream("student.ser");
+        ObjectInputStream ois = new ObjectInputStream(fis);
+        Student s2 = (Student) ois.readObject();
+        ois.close();
+        System.out.println("Object Deserialize झाला: " + s2.name);
+    }
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +632,23 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -482,7 +675,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -492,9 +685,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -516,6 +706,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C8631A7-75D6-403D-95BF-04DB55FBFC7E}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -847,27 +1046,27 @@
     <col min="6" max="6" width="74.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5"/>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:6" s="5" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -877,11 +1076,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -891,14 +1090,14 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="6" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="76.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -911,9 +1110,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:6" s="5" customFormat="1" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -929,9 +1128,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -947,9 +1146,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="6" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
-      <c r="B7" s="5" t="s">
+    <row r="7" spans="1:6" s="5" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -965,9 +1164,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:6" s="5" customFormat="1" ht="112.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -983,9 +1182,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="6" customFormat="1" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="5" t="s">
+    <row r="9" spans="1:6" s="5" customFormat="1" ht="85.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1046,7 +1245,7 @@
       <c r="D12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1065,12 +1264,38 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="3" customFormat="1" ht="286.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="3" customFormat="1" ht="100.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="C15" s="4"/>
+      <c r="B15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>

</xml_diff>